<commit_message>
agregada opciones de dibujo en patrón de radiación
</commit_message>
<xml_diff>
--- a/resultsUTM.xlsx
+++ b/resultsUTM.xlsx
@@ -479,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,20 +504,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>166021.4430805406</v>
-      </c>
-      <c r="D2" t="n">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -529,7 +515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -552,20 +538,6 @@
         <is>
           <t>Huso</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>166021.4430805406</v>
-      </c>
-      <c r="D2" t="n">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
customización del perímetro de radiación
</commit_message>
<xml_diff>
--- a/resultsUTM.xlsx
+++ b/resultsUTM.xlsx
@@ -642,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10.49011413959285</v>
+        <v>10.53368243087264</v>
       </c>
       <c r="C2" t="n">
         <v>-66.8894638888889</v>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -659,16 +659,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>10.49018213513634</v>
+        <v>10.52857664048812</v>
       </c>
       <c r="C3" t="n">
-        <v>-66.88921006114315</v>
+        <v>-66.88232409661181</v>
       </c>
       <c r="D3" t="n">
         <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>0.16</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="4">
@@ -676,16 +676,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10.49020170464005</v>
+        <v>10.52253203210929</v>
       </c>
       <c r="C4" t="n">
-        <v>-66.88893269934989</v>
+        <v>-66.87696400422162</v>
       </c>
       <c r="D4" t="n">
         <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>0.17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -693,16 +693,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>10.49016700055255</v>
+        <v>10.52377437938858</v>
       </c>
       <c r="C5" t="n">
-        <v>-66.88864166258092</v>
+        <v>-66.86890599615849</v>
       </c>
       <c r="D5" t="n">
         <v>30</v>
       </c>
       <c r="E5" t="n">
-        <v>0.18</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="6">
@@ -710,16 +710,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>10.49007414864192</v>
+        <v>10.52317278993719</v>
       </c>
       <c r="C6" t="n">
-        <v>-66.88834813135929</v>
+        <v>-66.86009870446183</v>
       </c>
       <c r="D6" t="n">
         <v>40</v>
       </c>
       <c r="E6" t="n">
-        <v>0.19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -727,16 +727,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>10.48992151547469</v>
+        <v>10.50608875571192</v>
       </c>
       <c r="C7" t="n">
-        <v>-66.888064196901</v>
+        <v>-66.86846741155375</v>
       </c>
       <c r="D7" t="n">
         <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -744,16 +744,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>10.48962904573469</v>
+        <v>10.50224051548196</v>
       </c>
       <c r="C8" t="n">
-        <v>-66.88794481127285</v>
+        <v>-66.86572733339695</v>
       </c>
       <c r="D8" t="n">
         <v>60</v>
       </c>
       <c r="E8" t="n">
-        <v>0.192</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -761,16 +761,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>10.48931969839657</v>
+        <v>10.49798288788125</v>
       </c>
       <c r="C9" t="n">
-        <v>-66.88791861313142</v>
+        <v>-66.86370857171558</v>
       </c>
       <c r="D9" t="n">
         <v>70</v>
       </c>
       <c r="E9" t="n">
-        <v>0.18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -778,16 +778,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>10.48903184739289</v>
+        <v>10.49344525284491</v>
       </c>
       <c r="C10" t="n">
-        <v>-66.88793439535173</v>
+        <v>-66.86247244145667</v>
       </c>
       <c r="D10" t="n">
         <v>80</v>
       </c>
       <c r="E10" t="n">
-        <v>0.17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -795,16 +795,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10.48876666332905</v>
+        <v>10.48876549328599</v>
       </c>
       <c r="C11" t="n">
-        <v>-66.88800215984465</v>
+        <v>-66.86205646937798</v>
       </c>
       <c r="D11" t="n">
         <v>90</v>
       </c>
       <c r="E11" t="n">
-        <v>0.16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -812,16 +812,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>10.48853267760361</v>
+        <v>10.48330543959474</v>
       </c>
       <c r="C12" t="n">
-        <v>-66.88811433794461</v>
+        <v>-66.85797489857073</v>
       </c>
       <c r="D12" t="n">
         <v>100</v>
       </c>
       <c r="E12" t="n">
-        <v>0.15</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="13">
@@ -829,16 +829,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>10.48833652571914</v>
+        <v>10.4783191109526</v>
       </c>
       <c r="C13" t="n">
-        <v>-66.88826201156242</v>
+        <v>-66.8602763839254</v>
       </c>
       <c r="D13" t="n">
         <v>110</v>
       </c>
       <c r="E13" t="n">
-        <v>0.14</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="14">
@@ -846,16 +846,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>10.4881378440513</v>
+        <v>10.47079879745071</v>
       </c>
       <c r="C14" t="n">
-        <v>-66.88835623346441</v>
+        <v>-66.85781836294359</v>
       </c>
       <c r="D14" t="n">
         <v>120</v>
       </c>
       <c r="E14" t="n">
-        <v>0.14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -863,16 +863,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>10.48792939745352</v>
+        <v>10.47202067151893</v>
       </c>
       <c r="C15" t="n">
-        <v>-66.88844911872984</v>
+        <v>-66.86916952834326</v>
       </c>
       <c r="D15" t="n">
         <v>130</v>
       </c>
       <c r="E15" t="n">
-        <v>0.145</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="16">
@@ -880,16 +880,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>10.48773444130732</v>
+        <v>10.47156259440271</v>
       </c>
       <c r="C16" t="n">
-        <v>-66.8885830343408</v>
+        <v>-66.87478374641827</v>
       </c>
       <c r="D16" t="n">
         <v>140</v>
       </c>
       <c r="E16" t="n">
-        <v>0.15</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="17">
@@ -897,16 +897,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>10.48728853416244</v>
+        <v>10.46542745785906</v>
       </c>
       <c r="C17" t="n">
-        <v>-66.88859599141392</v>
+        <v>-66.87576121171743</v>
       </c>
       <c r="D17" t="n">
         <v>150</v>
       </c>
       <c r="E17" t="n">
-        <v>0.19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -914,16 +914,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>10.4875004559581</v>
+        <v>10.46344232221885</v>
       </c>
       <c r="C18" t="n">
-        <v>-66.8889951963278</v>
+        <v>-66.88009076569712</v>
       </c>
       <c r="D18" t="n">
         <v>160</v>
       </c>
       <c r="E18" t="n">
-        <v>0.15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -931,16 +931,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>10.48752813159059</v>
+        <v>10.45337988958488</v>
       </c>
       <c r="C19" t="n">
-        <v>-66.88924179151601</v>
+        <v>-66.88311894896212</v>
       </c>
       <c r="D19" t="n">
         <v>170</v>
       </c>
       <c r="E19" t="n">
-        <v>0.14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -948,7 +948,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>10.48831750902461</v>
+        <v>10.45283405530189</v>
       </c>
       <c r="C20" t="n">
         <v>-66.8894638888889</v>
@@ -957,7 +957,7 @@
         <v>180</v>
       </c>
       <c r="E20" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -965,16 +965,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>10.48832433272861</v>
+        <v>10.45161054743679</v>
       </c>
       <c r="C21" t="n">
-        <v>-66.88954320958328</v>
+        <v>-66.89612603781465</v>
       </c>
       <c r="D21" t="n">
         <v>190</v>
       </c>
       <c r="E21" t="n">
-        <v>0.05</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="22">
@@ -982,16 +982,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>10.48876666666667</v>
+        <v>10.44824758408166</v>
       </c>
       <c r="C22" t="n">
-        <v>-66.8894638888889</v>
+        <v>-66.90446015129913</v>
       </c>
       <c r="D22" t="n">
         <v>200</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="23">
@@ -999,16 +999,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>10.48837768465685</v>
+        <v>10.45764759146022</v>
       </c>
       <c r="C23" t="n">
-        <v>-66.889692283765</v>
+        <v>-66.90773366666599</v>
       </c>
       <c r="D23" t="n">
         <v>210</v>
       </c>
       <c r="E23" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1016,16 +1016,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>10.48842259181621</v>
+        <v>10.46123982833683</v>
       </c>
       <c r="C24" t="n">
-        <v>-66.88975750772445</v>
+        <v>-66.91295133456889</v>
       </c>
       <c r="D24" t="n">
         <v>220</v>
       </c>
       <c r="E24" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1033,16 +1033,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>10.48795826885925</v>
+        <v>10.47144320048521</v>
       </c>
       <c r="C25" t="n">
-        <v>-66.89044366706491</v>
+        <v>-66.91045801584175</v>
       </c>
       <c r="D25" t="n">
         <v>230</v>
       </c>
       <c r="E25" t="n">
-        <v>0.14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1050,16 +1050,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>10.48809292800354</v>
+        <v>10.47529105778028</v>
       </c>
       <c r="C26" t="n">
-        <v>-66.89065066238578</v>
+        <v>-66.91319837748942</v>
       </c>
       <c r="D26" t="n">
         <v>240</v>
       </c>
       <c r="E26" t="n">
-        <v>0.15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1067,16 +1067,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>10.48832116345898</v>
+        <v>10.48262136782188</v>
       </c>
       <c r="C27" t="n">
-        <v>-66.89070869034383</v>
+        <v>-66.90663324798888</v>
       </c>
       <c r="D27" t="n">
         <v>250</v>
       </c>
       <c r="E27" t="n">
-        <v>0.145</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1084,16 +1084,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>10.48853267760361</v>
+        <v>10.48564634470289</v>
       </c>
       <c r="C28" t="n">
-        <v>-66.8908134398332</v>
+        <v>-66.90745773368864</v>
       </c>
       <c r="D28" t="n">
         <v>260</v>
       </c>
       <c r="E28" t="n">
-        <v>0.15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1101,16 +1101,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>10.48876666332905</v>
+        <v>10.48876653629103</v>
       </c>
       <c r="C29" t="n">
-        <v>-66.89092561793316</v>
+        <v>-66.89859969541307</v>
       </c>
       <c r="D29" t="n">
         <v>270</v>
       </c>
       <c r="E29" t="n">
-        <v>0.16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1118,16 +1118,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>10.48903184739289</v>
+        <v>10.49110624432473</v>
       </c>
       <c r="C30" t="n">
-        <v>-66.89099338242607</v>
+        <v>-66.90295951057013</v>
       </c>
       <c r="D30" t="n">
         <v>280</v>
       </c>
       <c r="E30" t="n">
-        <v>0.17</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31">
@@ -1135,16 +1135,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>10.48931969839657</v>
+        <v>10.49183897075209</v>
       </c>
       <c r="C31" t="n">
-        <v>-66.89100916464639</v>
+        <v>-66.89804882410189</v>
       </c>
       <c r="D31" t="n">
         <v>290</v>
       </c>
       <c r="E31" t="n">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1152,16 +1152,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>10.48962006265655</v>
+        <v>10.49550381123731</v>
       </c>
       <c r="C32" t="n">
-        <v>-66.89096714273616</v>
+        <v>-66.90133190810936</v>
       </c>
       <c r="D32" t="n">
         <v>300</v>
       </c>
       <c r="E32" t="n">
-        <v>0.19</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="33">
@@ -1169,16 +1169,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>10.48980603086934</v>
+        <v>10.49454084948603</v>
       </c>
       <c r="C33" t="n">
-        <v>-66.89072361120792</v>
+        <v>-66.89646245331389</v>
       </c>
       <c r="D33" t="n">
         <v>310</v>
       </c>
       <c r="E33" t="n">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1186,16 +1186,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>10.48993651914348</v>
+        <v>10.50941066445419</v>
       </c>
       <c r="C34" t="n">
-        <v>-66.89046219781351</v>
+        <v>-66.90708221462212</v>
       </c>
       <c r="D34" t="n">
         <v>320</v>
       </c>
       <c r="E34" t="n">
-        <v>0.17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1203,16 +1203,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>10.49001140800288</v>
+        <v>10.51988469886784</v>
       </c>
       <c r="C35" t="n">
-        <v>-66.89019475635075</v>
+        <v>-66.90773734114036</v>
       </c>
       <c r="D35" t="n">
         <v>330</v>
       </c>
       <c r="E35" t="n">
-        <v>0.16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1220,16 +1220,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>10.49007508367786</v>
+        <v>10.51409073659551</v>
       </c>
       <c r="C36" t="n">
-        <v>-66.88994820856453</v>
+        <v>-66.89883854618395</v>
       </c>
       <c r="D36" t="n">
         <v>340</v>
       </c>
       <c r="E36" t="n">
-        <v>0.155</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1237,16 +1237,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>10.490120208395</v>
+        <v>10.52415331794662</v>
       </c>
       <c r="C37" t="n">
-        <v>-66.88970661162223</v>
+        <v>-66.8958102799791</v>
       </c>
       <c r="D37" t="n">
         <v>350</v>
       </c>
       <c r="E37" t="n">
-        <v>0.153</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -1254,7 +1254,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>10.49011413959285</v>
+        <v>10.53368243087264</v>
       </c>
       <c r="C38" t="n">
         <v>-66.8894638888889</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>0.15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1317,10 +1317,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1160376.90987259</v>
+        <v>1165197.197817992</v>
       </c>
       <c r="C2" t="n">
-        <v>730999.3622942066</v>
+        <v>730966.9535116111</v>
       </c>
       <c r="D2" t="n">
         <v>19</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -1337,10 +1337,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1160384.619218405</v>
+        <v>1164637.578002534</v>
       </c>
       <c r="C3" t="n">
-        <v>731027.1052199232</v>
+        <v>731752.4497410624</v>
       </c>
       <c r="D3" t="n">
         <v>19</v>
@@ -1349,7 +1349,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>0.16</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="4">
@@ -1357,10 +1357,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>1160386.988151005</v>
+        <v>1163972.782121793</v>
       </c>
       <c r="C4" t="n">
-        <v>731057.4610052236</v>
+        <v>732343.8239250184</v>
       </c>
       <c r="D4" t="n">
         <v>19</v>
@@ -1369,7 +1369,7 @@
         <v>20</v>
       </c>
       <c r="F4" t="n">
-        <v>0.17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -1377,10 +1377,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>1160383.362470218</v>
+        <v>1164116.218326742</v>
       </c>
       <c r="C5" t="n">
-        <v>731089.3544676575</v>
+        <v>733225.1350259718</v>
       </c>
       <c r="D5" t="n">
         <v>19</v>
@@ -1389,7 +1389,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="n">
-        <v>0.18</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="6">
@@ -1397,10 +1397,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>1160373.305323246</v>
+        <v>1164056.226077507</v>
       </c>
       <c r="C6" t="n">
-        <v>731121.5642663511</v>
+        <v>734189.8722406242</v>
       </c>
       <c r="D6" t="n">
         <v>19</v>
@@ -1409,7 +1409,7 @@
         <v>40</v>
       </c>
       <c r="F6" t="n">
-        <v>0.19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -1417,10 +1417,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>1160356.627099485</v>
+        <v>1162159.825806272</v>
       </c>
       <c r="C7" t="n">
-        <v>731152.767676768</v>
+        <v>733286.4447887306</v>
       </c>
       <c r="D7" t="n">
         <v>19</v>
@@ -1429,7 +1429,7 @@
         <v>50</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -1437,10 +1437,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>1160324.356750412</v>
+        <v>1161736.097501346</v>
       </c>
       <c r="C8" t="n">
-        <v>731166.0573387045</v>
+        <v>733589.3567908132</v>
       </c>
       <c r="D8" t="n">
         <v>19</v>
@@ -1449,7 +1449,7 @@
         <v>60</v>
       </c>
       <c r="F8" t="n">
-        <v>0.192</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1457,10 +1457,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>1160290.150596581</v>
+        <v>1161266.53928228</v>
       </c>
       <c r="C9" t="n">
-        <v>731169.1557611845</v>
+        <v>733813.6023235838</v>
       </c>
       <c r="D9" t="n">
         <v>19</v>
@@ -1469,7 +1469,7 @@
         <v>70</v>
       </c>
       <c r="F9" t="n">
-        <v>0.18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
@@ -1477,10 +1477,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>1160258.291881</v>
+        <v>1160765.418966625</v>
       </c>
       <c r="C10" t="n">
-        <v>731167.641466193</v>
+        <v>733952.3671894547</v>
       </c>
       <c r="D10" t="n">
         <v>19</v>
@@ -1489,7 +1489,7 @@
         <v>80</v>
       </c>
       <c r="F10" t="n">
-        <v>0.17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -1497,10 +1497,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>1160228.902766971</v>
+        <v>1160247.963548178</v>
       </c>
       <c r="C11" t="n">
-        <v>731160.4183871776</v>
+        <v>734001.4346960919</v>
       </c>
       <c r="D11" t="n">
         <v>19</v>
@@ -1509,7 +1509,7 @@
         <v>90</v>
       </c>
       <c r="F11" t="n">
-        <v>0.16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -1517,10 +1517,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>1160202.932716269</v>
+        <v>1159646.90621188</v>
       </c>
       <c r="C12" t="n">
-        <v>731148.3089288148</v>
+        <v>734452.4770937982</v>
       </c>
       <c r="D12" t="n">
         <v>19</v>
@@ -1529,7 +1529,7 @@
         <v>100</v>
       </c>
       <c r="F12" t="n">
-        <v>0.15</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="13">
@@ -1537,10 +1537,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>1160181.122425196</v>
+        <v>1159093.508110695</v>
       </c>
       <c r="C13" t="n">
-        <v>731132.2846699218</v>
+        <v>734204.2104602387</v>
       </c>
       <c r="D13" t="n">
         <v>19</v>
@@ -1549,7 +1549,7 @@
         <v>110</v>
       </c>
       <c r="F13" t="n">
-        <v>0.14</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="14">
@@ -1557,10 +1557,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>1160159.071540345</v>
+        <v>1158263.294866764</v>
       </c>
       <c r="C14" t="n">
-        <v>731122.1151175372</v>
+        <v>734479.0300465914</v>
       </c>
       <c r="D14" t="n">
         <v>19</v>
@@ -1569,7 +1569,7 @@
         <v>120</v>
       </c>
       <c r="F14" t="n">
-        <v>0.14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -1577,10 +1577,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>1160135.941276675</v>
+        <v>1158390.053822168</v>
       </c>
       <c r="C15" t="n">
-        <v>731112.0991596049</v>
+        <v>733235.099177414</v>
       </c>
       <c r="D15" t="n">
         <v>19</v>
@@ -1589,7 +1589,7 @@
         <v>130</v>
       </c>
       <c r="F15" t="n">
-        <v>0.145</v>
+        <v>2.9</v>
       </c>
     </row>
     <row r="16">
@@ -1597,10 +1597,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>1160114.273417147</v>
+        <v>1158335.220876137</v>
       </c>
       <c r="C16" t="n">
-        <v>731097.5804277167</v>
+        <v>732620.6580264606</v>
       </c>
       <c r="D16" t="n">
         <v>19</v>
@@ -1609,7 +1609,7 @@
         <v>140</v>
       </c>
       <c r="F16" t="n">
-        <v>0.15</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="17">
@@ -1617,10 +1617,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>1160064.929872107</v>
+        <v>1157655.718755977</v>
       </c>
       <c r="C17" t="n">
-        <v>731096.4927223135</v>
+        <v>732518.1957138145</v>
       </c>
       <c r="D17" t="n">
         <v>19</v>
@@ -1629,7 +1629,7 @@
         <v>150</v>
       </c>
       <c r="F17" t="n">
-        <v>0.19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
@@ -1637,10 +1637,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>1160088.083042928</v>
+        <v>1157432.896478269</v>
       </c>
       <c r="C18" t="n">
-        <v>731052.6232094876</v>
+        <v>732045.5577147251</v>
       </c>
       <c r="D18" t="n">
         <v>19</v>
@@ -1649,7 +1649,7 @@
         <v>160</v>
       </c>
       <c r="F18" t="n">
-        <v>0.15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1657,10 +1657,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>1160090.96384623</v>
+        <v>1156317.385136057</v>
       </c>
       <c r="C19" t="n">
-        <v>731025.6009736815</v>
+        <v>731721.4201896497</v>
       </c>
       <c r="D19" t="n">
         <v>19</v>
@@ -1669,7 +1669,7 @@
         <v>170</v>
       </c>
       <c r="F19" t="n">
-        <v>0.14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1677,10 +1677,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>1160178.135356737</v>
+        <v>1156252.342631783</v>
       </c>
       <c r="C20" t="n">
-        <v>731000.6958858003</v>
+        <v>731026.9880103853</v>
       </c>
       <c r="D20" t="n">
         <v>19</v>
@@ -1689,7 +1689,7 @@
         <v>180</v>
       </c>
       <c r="F20" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1697,10 +1697,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>1160178.832048311</v>
+        <v>1156112.107477938</v>
       </c>
       <c r="C21" t="n">
-        <v>730992.005384289</v>
+        <v>730298.3181538805</v>
       </c>
       <c r="D21" t="n">
         <v>19</v>
@@ -1709,7 +1709,7 @@
         <v>190</v>
       </c>
       <c r="F21" t="n">
-        <v>0.05</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="22">
@@ -1717,10 +1717,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>1160227.828983885</v>
+        <v>1155733.972035679</v>
       </c>
       <c r="C22" t="n">
-        <v>731000.3625090888</v>
+        <v>729388.1191171468</v>
       </c>
       <c r="D22" t="n">
         <v>19</v>
@@ -1729,7 +1729,7 @@
         <v>200</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="23">
@@ -1737,10 +1737,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>1160184.625268458</v>
+        <v>1156771.573915364</v>
       </c>
       <c r="C23" t="n">
-        <v>730975.6425050055</v>
+        <v>729022.7408273679</v>
       </c>
       <c r="D23" t="n">
         <v>19</v>
@@ -1749,7 +1749,7 @@
         <v>210</v>
       </c>
       <c r="F23" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1757,10 +1757,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>1160189.545772638</v>
+        <v>1157165.21924914</v>
       </c>
       <c r="C24" t="n">
-        <v>730968.4673047503</v>
+        <v>728448.7395309911</v>
       </c>
       <c r="D24" t="n">
         <v>19</v>
@@ -1769,7 +1769,7 @@
         <v>220</v>
       </c>
       <c r="F24" t="n">
-        <v>0.05</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -1777,10 +1777,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>1160137.670444666</v>
+        <v>1158295.885742532</v>
       </c>
       <c r="C25" t="n">
-        <v>730893.6789186327</v>
+        <v>728714.2904084951</v>
       </c>
       <c r="D25" t="n">
         <v>19</v>
@@ -1789,7 +1789,7 @@
         <v>230</v>
       </c>
       <c r="F25" t="n">
-        <v>0.14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
@@ -1797,10 +1797,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>1160152.416800764</v>
+        <v>1158719.607649517</v>
       </c>
       <c r="C26" t="n">
-        <v>730870.9134997089</v>
+        <v>728411.3949831483</v>
       </c>
       <c r="D26" t="n">
         <v>19</v>
@@ -1809,7 +1809,7 @@
         <v>240</v>
       </c>
       <c r="F26" t="n">
-        <v>0.15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27">
@@ -1817,10 +1817,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>1160177.625555494</v>
+        <v>1159535.37519962</v>
       </c>
       <c r="C27" t="n">
-        <v>730864.390272224</v>
+        <v>729124.891630362</v>
       </c>
       <c r="D27" t="n">
         <v>19</v>
@@ -1829,7 +1829,7 @@
         <v>250</v>
       </c>
       <c r="F27" t="n">
-        <v>0.145</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1837,10 +1837,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>1160200.950010203</v>
+        <v>1159869.446756123</v>
       </c>
       <c r="C28" t="n">
-        <v>730852.7635592273</v>
+        <v>729032.3864964311</v>
       </c>
       <c r="D28" t="n">
         <v>19</v>
@@ -1849,7 +1849,7 @@
         <v>260</v>
       </c>
       <c r="F28" t="n">
-        <v>0.15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1857,10 +1857,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>1160226.755207589</v>
+        <v>1160221.117993379</v>
       </c>
       <c r="C29" t="n">
-        <v>730840.3067773966</v>
+        <v>730000.0165838246</v>
       </c>
       <c r="D29" t="n">
         <v>19</v>
@@ -1869,7 +1869,7 @@
         <v>270</v>
       </c>
       <c r="F29" t="n">
-        <v>0.16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
@@ -1877,10 +1877,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>1160256.044708366</v>
+        <v>1160476.789595093</v>
       </c>
       <c r="C30" t="n">
-        <v>730832.6900452506</v>
+        <v>729520.9049045217</v>
       </c>
       <c r="D30" t="n">
         <v>19</v>
@@ -1889,7 +1889,7 @@
         <v>280</v>
       </c>
       <c r="F30" t="n">
-        <v>0.17</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="31">
@@ -1897,10 +1897,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>1160287.880176784</v>
+        <v>1160561.445345811</v>
       </c>
       <c r="C31" t="n">
-        <v>730830.7484266341</v>
+        <v>730058.0638181781</v>
       </c>
       <c r="D31" t="n">
         <v>19</v>
@@ -1909,7 +1909,7 @@
         <v>290</v>
       </c>
       <c r="F31" t="n">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
@@ -1917,10 +1917,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>1160321.142512976</v>
+        <v>1160964.510227983</v>
       </c>
       <c r="C32" t="n">
-        <v>730835.126913348</v>
+        <v>729695.8736891557</v>
       </c>
       <c r="D32" t="n">
         <v>19</v>
@@ -1929,7 +1929,7 @@
         <v>300</v>
       </c>
       <c r="F32" t="n">
-        <v>0.19</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="33">
@@ -1937,10 +1937,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>1160341.896329164</v>
+        <v>1160861.534311408</v>
       </c>
       <c r="C33" t="n">
-        <v>730861.6549696039</v>
+        <v>730229.7654407904</v>
       </c>
       <c r="D33" t="n">
         <v>19</v>
@@ -1949,7 +1949,7 @@
         <v>310</v>
       </c>
       <c r="F33" t="n">
-        <v>0.18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1957,10 +1957,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>1160356.525151304</v>
+        <v>1162498.915800803</v>
       </c>
       <c r="C34" t="n">
-        <v>730890.1821724179</v>
+        <v>729055.9991283424</v>
       </c>
       <c r="D34" t="n">
         <v>19</v>
@@ -1969,7 +1969,7 @@
         <v>320</v>
       </c>
       <c r="F34" t="n">
-        <v>0.17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1977,10 +1977,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>1160365.007057462</v>
+        <v>1163657.246433939</v>
       </c>
       <c r="C35" t="n">
-        <v>730919.4106692676</v>
+        <v>728976.5442736079</v>
       </c>
       <c r="D35" t="n">
         <v>19</v>
@@ -1989,7 +1989,7 @@
         <v>330</v>
       </c>
       <c r="F35" t="n">
-        <v>0.16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1997,10 +1997,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>1160372.233047347</v>
+        <v>1163022.732732167</v>
       </c>
       <c r="C36" t="n">
-        <v>730946.3596815391</v>
+        <v>729955.1277799493</v>
       </c>
       <c r="D36" t="n">
         <v>19</v>
@@ -2009,7 +2009,7 @@
         <v>340</v>
       </c>
       <c r="F36" t="n">
-        <v>0.155</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -2017,10 +2017,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>1160377.402994306</v>
+        <v>1164138.249365305</v>
       </c>
       <c r="C37" t="n">
-        <v>730972.7803529748</v>
+        <v>730279.2193067948</v>
       </c>
       <c r="D37" t="n">
         <v>19</v>
@@ -2029,7 +2029,7 @@
         <v>350</v>
       </c>
       <c r="F37" t="n">
-        <v>0.153</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
@@ -2037,10 +2037,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>1160376.90987259</v>
+        <v>1165197.197817992</v>
       </c>
       <c r="C38" t="n">
-        <v>730999.3622942066</v>
+        <v>730966.9535116111</v>
       </c>
       <c r="D38" t="n">
         <v>19</v>
@@ -2049,7 +2049,7 @@
         <v>0</v>
       </c>
       <c r="F38" t="n">
-        <v>0.15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregada opción para cambiar color de marcadores en Localización
</commit_message>
<xml_diff>
--- a/resultsUTM.xlsx
+++ b/resultsUTM.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,20 @@
         <v>731000.3625090888</v>
       </c>
       <c r="D2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1160227.639225001</v>
+      </c>
+      <c r="C3" t="n">
+        <v>730972.0756343598</v>
+      </c>
+      <c r="D3" t="n">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
visual changes on coordinates and message of lenght in spanish
</commit_message>
<xml_diff>
--- a/resultsUTM.xlsx
+++ b/resultsUTM.xlsx
@@ -473,10 +473,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1160227.639225001</v>
+        <v>1160395.180980101</v>
       </c>
       <c r="C3" t="n">
-        <v>730972.0756343598</v>
+        <v>754726.4470557353</v>
       </c>
       <c r="D3" t="n">
         <v>19</v>
@@ -493,7 +493,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,34 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1160227.828983885</v>
+      </c>
+      <c r="C2" t="n">
+        <v>731000.3625090888</v>
+      </c>
+      <c r="D2" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1160395.180980101</v>
+      </c>
+      <c r="C3" t="n">
+        <v>754726.4470557353</v>
+      </c>
+      <c r="D3" t="n">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -529,7 +557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,6 +596,20 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1160395.180980101</v>
+      </c>
+      <c r="C3" t="n">
+        <v>754726.4470557353</v>
+      </c>
+      <c r="D3" t="n">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -579,7 +621,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1238,6 +1280,635 @@
         <v>5</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>10.53368243087264</v>
+      </c>
+      <c r="C39" t="n">
+        <v>-66.67279722222223</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>10.52857664048812</v>
+      </c>
+      <c r="C40" t="n">
+        <v>-66.66565742994513</v>
+      </c>
+      <c r="D40" t="n">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>10.52253203210929</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-66.66029733755495</v>
+      </c>
+      <c r="D41" t="n">
+        <v>20</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>10.52377437938858</v>
+      </c>
+      <c r="C42" t="n">
+        <v>-66.65223932949182</v>
+      </c>
+      <c r="D42" t="n">
+        <v>30</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>10.52317278993719</v>
+      </c>
+      <c r="C43" t="n">
+        <v>-66.64343203779517</v>
+      </c>
+      <c r="D43" t="n">
+        <v>40</v>
+      </c>
+      <c r="E43" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>10.50608875571192</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-66.65180074488707</v>
+      </c>
+      <c r="D44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>10.50224051548196</v>
+      </c>
+      <c r="C45" t="n">
+        <v>-66.64906066673028</v>
+      </c>
+      <c r="D45" t="n">
+        <v>60</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>10.49798288788125</v>
+      </c>
+      <c r="C46" t="n">
+        <v>-66.64704190504889</v>
+      </c>
+      <c r="D46" t="n">
+        <v>70</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>10.49344525284491</v>
+      </c>
+      <c r="C47" t="n">
+        <v>-66.64580577478999</v>
+      </c>
+      <c r="D47" t="n">
+        <v>80</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>10.48876549328599</v>
+      </c>
+      <c r="C48" t="n">
+        <v>-66.64538980271131</v>
+      </c>
+      <c r="D48" t="n">
+        <v>90</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>10.48330543959474</v>
+      </c>
+      <c r="C49" t="n">
+        <v>-66.64130823190406</v>
+      </c>
+      <c r="D49" t="n">
+        <v>100</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>10.4783191109526</v>
+      </c>
+      <c r="C50" t="n">
+        <v>-66.64360971725871</v>
+      </c>
+      <c r="D50" t="n">
+        <v>110</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>10.47079879745071</v>
+      </c>
+      <c r="C51" t="n">
+        <v>-66.64115169627692</v>
+      </c>
+      <c r="D51" t="n">
+        <v>120</v>
+      </c>
+      <c r="E51" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>10.47202067151893</v>
+      </c>
+      <c r="C52" t="n">
+        <v>-66.6525028616766</v>
+      </c>
+      <c r="D52" t="n">
+        <v>130</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>10.47156259440271</v>
+      </c>
+      <c r="C53" t="n">
+        <v>-66.65811707975161</v>
+      </c>
+      <c r="D53" t="n">
+        <v>140</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>10.46542745785906</v>
+      </c>
+      <c r="C54" t="n">
+        <v>-66.65909454505076</v>
+      </c>
+      <c r="D54" t="n">
+        <v>150</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>10.46344232221885</v>
+      </c>
+      <c r="C55" t="n">
+        <v>-66.66342409903044</v>
+      </c>
+      <c r="D55" t="n">
+        <v>160</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>10.45337988958488</v>
+      </c>
+      <c r="C56" t="n">
+        <v>-66.66645228229544</v>
+      </c>
+      <c r="D56" t="n">
+        <v>170</v>
+      </c>
+      <c r="E56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>10.45283405530189</v>
+      </c>
+      <c r="C57" t="n">
+        <v>-66.67279722222223</v>
+      </c>
+      <c r="D57" t="n">
+        <v>180</v>
+      </c>
+      <c r="E57" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>10.45161054743679</v>
+      </c>
+      <c r="C58" t="n">
+        <v>-66.67945937114798</v>
+      </c>
+      <c r="D58" t="n">
+        <v>190</v>
+      </c>
+      <c r="E58" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>10.44824758408166</v>
+      </c>
+      <c r="C59" t="n">
+        <v>-66.68779348463246</v>
+      </c>
+      <c r="D59" t="n">
+        <v>200</v>
+      </c>
+      <c r="E59" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>10.45764759146022</v>
+      </c>
+      <c r="C60" t="n">
+        <v>-66.69106699999932</v>
+      </c>
+      <c r="D60" t="n">
+        <v>210</v>
+      </c>
+      <c r="E60" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>10.46123982833683</v>
+      </c>
+      <c r="C61" t="n">
+        <v>-66.69628466790221</v>
+      </c>
+      <c r="D61" t="n">
+        <v>220</v>
+      </c>
+      <c r="E61" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>10.47144320048521</v>
+      </c>
+      <c r="C62" t="n">
+        <v>-66.69379134917509</v>
+      </c>
+      <c r="D62" t="n">
+        <v>230</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>10.47529105778028</v>
+      </c>
+      <c r="C63" t="n">
+        <v>-66.69653171082275</v>
+      </c>
+      <c r="D63" t="n">
+        <v>240</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>10.48262136782188</v>
+      </c>
+      <c r="C64" t="n">
+        <v>-66.68996658132221</v>
+      </c>
+      <c r="D64" t="n">
+        <v>250</v>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>10.48564634470289</v>
+      </c>
+      <c r="C65" t="n">
+        <v>-66.69079106702196</v>
+      </c>
+      <c r="D65" t="n">
+        <v>260</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>10.48876653629103</v>
+      </c>
+      <c r="C66" t="n">
+        <v>-66.6819330287464</v>
+      </c>
+      <c r="D66" t="n">
+        <v>270</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>10.49110624432473</v>
+      </c>
+      <c r="C67" t="n">
+        <v>-66.68629284390344</v>
+      </c>
+      <c r="D67" t="n">
+        <v>280</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>10.49183897075209</v>
+      </c>
+      <c r="C68" t="n">
+        <v>-66.68138215743522</v>
+      </c>
+      <c r="D68" t="n">
+        <v>290</v>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>10.49550381123731</v>
+      </c>
+      <c r="C69" t="n">
+        <v>-66.68466524144269</v>
+      </c>
+      <c r="D69" t="n">
+        <v>300</v>
+      </c>
+      <c r="E69" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>10.49454084948603</v>
+      </c>
+      <c r="C70" t="n">
+        <v>-66.67979578664722</v>
+      </c>
+      <c r="D70" t="n">
+        <v>310</v>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>10.50941066445419</v>
+      </c>
+      <c r="C71" t="n">
+        <v>-66.69041554795545</v>
+      </c>
+      <c r="D71" t="n">
+        <v>320</v>
+      </c>
+      <c r="E71" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>10.51988469886784</v>
+      </c>
+      <c r="C72" t="n">
+        <v>-66.69107067447369</v>
+      </c>
+      <c r="D72" t="n">
+        <v>330</v>
+      </c>
+      <c r="E72" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>10.51409073659551</v>
+      </c>
+      <c r="C73" t="n">
+        <v>-66.68217187951728</v>
+      </c>
+      <c r="D73" t="n">
+        <v>340</v>
+      </c>
+      <c r="E73" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>10.52415331794662</v>
+      </c>
+      <c r="C74" t="n">
+        <v>-66.67914361331242</v>
+      </c>
+      <c r="D74" t="n">
+        <v>350</v>
+      </c>
+      <c r="E74" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>10.53368243087264</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-66.67279722222223</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1249,7 +1920,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2024,6 +2695,746 @@
         <v>5</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>1165365.234029098</v>
+      </c>
+      <c r="C39" t="n">
+        <v>754689.5995655446</v>
+      </c>
+      <c r="D39" t="n">
+        <v>19</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>1164806.078225782</v>
+      </c>
+      <c r="C40" t="n">
+        <v>755475.5951735781</v>
+      </c>
+      <c r="D40" t="n">
+        <v>19</v>
+      </c>
+      <c r="E40" t="n">
+        <v>10</v>
+      </c>
+      <c r="F40" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1164141.596497289</v>
+      </c>
+      <c r="C41" t="n">
+        <v>756067.5138806826</v>
+      </c>
+      <c r="D41" t="n">
+        <v>19</v>
+      </c>
+      <c r="E41" t="n">
+        <v>20</v>
+      </c>
+      <c r="F41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>1164285.662934859</v>
+      </c>
+      <c r="C42" t="n">
+        <v>756948.8521218006</v>
+      </c>
+      <c r="D42" t="n">
+        <v>19</v>
+      </c>
+      <c r="E42" t="n">
+        <v>30</v>
+      </c>
+      <c r="F42" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>1164226.329457347</v>
+      </c>
+      <c r="C43" t="n">
+        <v>757913.7696892675</v>
+      </c>
+      <c r="D43" t="n">
+        <v>19</v>
+      </c>
+      <c r="E43" t="n">
+        <v>40</v>
+      </c>
+      <c r="F43" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>1162329.031729849</v>
+      </c>
+      <c r="C44" t="n">
+        <v>757011.5230327214</v>
+      </c>
+      <c r="D44" t="n">
+        <v>19</v>
+      </c>
+      <c r="E44" t="n">
+        <v>50</v>
+      </c>
+      <c r="F44" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1161905.451676256</v>
+      </c>
+      <c r="C45" t="n">
+        <v>757314.7711895413</v>
+      </c>
+      <c r="D45" t="n">
+        <v>19</v>
+      </c>
+      <c r="E45" t="n">
+        <v>60</v>
+      </c>
+      <c r="F45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>1161435.980664305</v>
+      </c>
+      <c r="C46" t="n">
+        <v>757539.3731267486</v>
+      </c>
+      <c r="D46" t="n">
+        <v>19</v>
+      </c>
+      <c r="E46" t="n">
+        <v>70</v>
+      </c>
+      <c r="F46" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>1160934.883913018</v>
+      </c>
+      <c r="C47" t="n">
+        <v>757678.5037528875</v>
+      </c>
+      <c r="D47" t="n">
+        <v>19</v>
+      </c>
+      <c r="E47" t="n">
+        <v>80</v>
+      </c>
+      <c r="F47" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>1160417.387770457</v>
+      </c>
+      <c r="C48" t="n">
+        <v>757727.9352189028</v>
+      </c>
+      <c r="D48" t="n">
+        <v>19</v>
+      </c>
+      <c r="E48" t="n">
+        <v>90</v>
+      </c>
+      <c r="F48" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>1159816.554667152</v>
+      </c>
+      <c r="C49" t="n">
+        <v>758179.4570319937</v>
+      </c>
+      <c r="D49" t="n">
+        <v>19</v>
+      </c>
+      <c r="E49" t="n">
+        <v>100</v>
+      </c>
+      <c r="F49" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1159262.905639278</v>
+      </c>
+      <c r="C50" t="n">
+        <v>757931.535880057</v>
+      </c>
+      <c r="D50" t="n">
+        <v>19</v>
+      </c>
+      <c r="E50" t="n">
+        <v>110</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>1158432.761823468</v>
+      </c>
+      <c r="C51" t="n">
+        <v>758206.9668368772</v>
+      </c>
+      <c r="D51" t="n">
+        <v>19</v>
+      </c>
+      <c r="E51" t="n">
+        <v>120</v>
+      </c>
+      <c r="F51" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>1158558.682693018</v>
+      </c>
+      <c r="C52" t="n">
+        <v>756962.769526904</v>
+      </c>
+      <c r="D52" t="n">
+        <v>19</v>
+      </c>
+      <c r="E52" t="n">
+        <v>130</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>1158503.418876175</v>
+      </c>
+      <c r="C53" t="n">
+        <v>756348.2779553839</v>
+      </c>
+      <c r="D53" t="n">
+        <v>19</v>
+      </c>
+      <c r="E53" t="n">
+        <v>140</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>1157823.748876176</v>
+      </c>
+      <c r="C54" t="n">
+        <v>756246.2686062483</v>
+      </c>
+      <c r="D54" t="n">
+        <v>19</v>
+      </c>
+      <c r="E54" t="n">
+        <v>150</v>
+      </c>
+      <c r="F54" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>1157600.569556579</v>
+      </c>
+      <c r="C55" t="n">
+        <v>755773.7162540231</v>
+      </c>
+      <c r="D55" t="n">
+        <v>19</v>
+      </c>
+      <c r="E55" t="n">
+        <v>160</v>
+      </c>
+      <c r="F55" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1156484.675957531</v>
+      </c>
+      <c r="C56" t="n">
+        <v>755450.2993892395</v>
+      </c>
+      <c r="D56" t="n">
+        <v>19</v>
+      </c>
+      <c r="E56" t="n">
+        <v>170</v>
+      </c>
+      <c r="F56" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1156419.146960565</v>
+      </c>
+      <c r="C57" t="n">
+        <v>754755.8128866819</v>
+      </c>
+      <c r="D57" t="n">
+        <v>19</v>
+      </c>
+      <c r="E57" t="n">
+        <v>180</v>
+      </c>
+      <c r="F57" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1156278.391168782</v>
+      </c>
+      <c r="C58" t="n">
+        <v>754027.1357930441</v>
+      </c>
+      <c r="D58" t="n">
+        <v>19</v>
+      </c>
+      <c r="E58" t="n">
+        <v>190</v>
+      </c>
+      <c r="F58" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>1155899.576852499</v>
+      </c>
+      <c r="C59" t="n">
+        <v>753117.0675596655</v>
+      </c>
+      <c r="D59" t="n">
+        <v>19</v>
+      </c>
+      <c r="E59" t="n">
+        <v>200</v>
+      </c>
+      <c r="F59" t="n">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1156937.074284995</v>
+      </c>
+      <c r="C60" t="n">
+        <v>752750.9246191554</v>
+      </c>
+      <c r="D60" t="n">
+        <v>19</v>
+      </c>
+      <c r="E60" t="n">
+        <v>210</v>
+      </c>
+      <c r="F60" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1157330.380457669</v>
+      </c>
+      <c r="C61" t="n">
+        <v>752176.5716975678</v>
+      </c>
+      <c r="D61" t="n">
+        <v>19</v>
+      </c>
+      <c r="E61" t="n">
+        <v>220</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1158461.389022815</v>
+      </c>
+      <c r="C62" t="n">
+        <v>752441.3820568862</v>
+      </c>
+      <c r="D62" t="n">
+        <v>19</v>
+      </c>
+      <c r="E62" t="n">
+        <v>230</v>
+      </c>
+      <c r="F62" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>1158884.962101866</v>
+      </c>
+      <c r="C63" t="n">
+        <v>752138.1522124861</v>
+      </c>
+      <c r="D63" t="n">
+        <v>19</v>
+      </c>
+      <c r="E63" t="n">
+        <v>240</v>
+      </c>
+      <c r="F63" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>1159701.336216117</v>
+      </c>
+      <c r="C64" t="n">
+        <v>752851.1875440651</v>
+      </c>
+      <c r="D64" t="n">
+        <v>19</v>
+      </c>
+      <c r="E64" t="n">
+        <v>250</v>
+      </c>
+      <c r="F64" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1160035.391197848</v>
+      </c>
+      <c r="C65" t="n">
+        <v>752758.4391027458</v>
+      </c>
+      <c r="D65" t="n">
+        <v>19</v>
+      </c>
+      <c r="E65" t="n">
+        <v>260</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>1160387.779281084</v>
+      </c>
+      <c r="C66" t="n">
+        <v>753725.963648667</v>
+      </c>
+      <c r="D66" t="n">
+        <v>19</v>
+      </c>
+      <c r="E66" t="n">
+        <v>270</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>1160643.156703452</v>
+      </c>
+      <c r="C67" t="n">
+        <v>753246.6078076609</v>
+      </c>
+      <c r="D67" t="n">
+        <v>19</v>
+      </c>
+      <c r="E67" t="n">
+        <v>280</v>
+      </c>
+      <c r="F67" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1160728.194916033</v>
+      </c>
+      <c r="C68" t="n">
+        <v>753783.7844191547</v>
+      </c>
+      <c r="D68" t="n">
+        <v>19</v>
+      </c>
+      <c r="E68" t="n">
+        <v>290</v>
+      </c>
+      <c r="F68" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>1161131.067059369</v>
+      </c>
+      <c r="C69" t="n">
+        <v>753421.2649247225</v>
+      </c>
+      <c r="D69" t="n">
+        <v>19</v>
+      </c>
+      <c r="E69" t="n">
+        <v>300</v>
+      </c>
+      <c r="F69" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1161028.444888703</v>
+      </c>
+      <c r="C70" t="n">
+        <v>753955.3033956827</v>
+      </c>
+      <c r="D70" t="n">
+        <v>19</v>
+      </c>
+      <c r="E70" t="n">
+        <v>310</v>
+      </c>
+      <c r="F70" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>1162665.247817952</v>
+      </c>
+      <c r="C71" t="n">
+        <v>752780.2405421536</v>
+      </c>
+      <c r="D71" t="n">
+        <v>19</v>
+      </c>
+      <c r="E71" t="n">
+        <v>320</v>
+      </c>
+      <c r="F71" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1163823.68705968</v>
+      </c>
+      <c r="C72" t="n">
+        <v>752699.9738486945</v>
+      </c>
+      <c r="D72" t="n">
+        <v>19</v>
+      </c>
+      <c r="E72" t="n">
+        <v>330</v>
+      </c>
+      <c r="F72" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>1163189.760149787</v>
+      </c>
+      <c r="C73" t="n">
+        <v>753679.1344290869</v>
+      </c>
+      <c r="D73" t="n">
+        <v>19</v>
+      </c>
+      <c r="E73" t="n">
+        <v>340</v>
+      </c>
+      <c r="F73" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>1164305.659088898</v>
+      </c>
+      <c r="C74" t="n">
+        <v>754002.5005536918</v>
+      </c>
+      <c r="D74" t="n">
+        <v>19</v>
+      </c>
+      <c r="E74" t="n">
+        <v>350</v>
+      </c>
+      <c r="F74" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>1165365.234029098</v>
+      </c>
+      <c r="C75" t="n">
+        <v>754689.5995655446</v>
+      </c>
+      <c r="D75" t="n">
+        <v>19</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>